<commit_message>
SoundBox Version Final 12.02.2014
</commit_message>
<xml_diff>
--- a/SoundBox/docs/Documento seguimiento tiempos y tareas.xlsx
+++ b/SoundBox/docs/Documento seguimiento tiempos y tareas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\Estructuras\SoundBox\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -144,7 +144,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="78">
   <si>
     <t>N13 - &lt;Título Ejercicio&gt;</t>
   </si>
@@ -360,6 +360,24 @@
   </si>
   <si>
     <t>N13 - Soundbox</t>
+  </si>
+  <si>
+    <t>Utilizamos un repositorio de Git que nos permitio aprender su manejo y la administracion de las distintas versiones de nuestro proyecto. Logramos distribuirnos bien las funciones, yo trabaje en el mundo, mi compañero en la interfaz. Esto permitio que no hubiera conflictos entre metodos y que lograramos entendernos a la hora de acoplar el projecto completo.</t>
+  </si>
+  <si>
+    <t>El manejo del tiempo es un factor muy complicado de administrar, en principio porque se le debe dedicar mucho tiempo a las distintas labores de desarrollo. Aun asi, logramos reunirnos frecuentemente para adelantar y ponernos de acuerdo en las decisiones del proyecto.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> En general me siento satisfecho con el resultado obtenido, sin embargo mejoraria el manejo del tiempo tanto mio como de trabajo en las horas libres con mi compañero.</t>
+  </si>
+  <si>
+    <t>Logramos definir el diseño del proyecto relativamente rápido y por esa razón la implementación del proyecto no fue compleja. Por otra parte el poder utilizar GIT para manejar el proyecto a distancia resultó muy util para poder trabajar en equipo y nos permitió acoplar fácilmente el proyecto.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Una de los elementos mas dificiles consistió en conseguir la librería adecuada que mejor se adecuara a la implementación del proyecto. Por otra parte, el manejo del tiempo fue una restricción complicada de manejar. </t>
+  </si>
+  <si>
+    <t>Poder utilizar y cuadrar el tiempo de una manera mas óptima y conseguir las librerías mas rápidamente.</t>
   </si>
 </sst>
 </file>
@@ -1641,7 +1659,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1828,10 +1846,13 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="69" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="69" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="38" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1899,6 +1920,102 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="AutoShape 5"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="AutoShape 5"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1932,6 +2049,102 @@
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>219075</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="AutoShape 5"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>219075</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="AutoShape 5"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
@@ -2215,8 +2428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40:H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2508,14 +2721,18 @@
       <c r="D14" s="15">
         <v>0</v>
       </c>
-      <c r="E14" s="34"/>
+      <c r="E14" s="34">
+        <v>6</v>
+      </c>
       <c r="F14" s="21">
         <v>2</v>
       </c>
       <c r="G14" s="15">
         <v>0</v>
       </c>
-      <c r="H14" s="34"/>
+      <c r="H14" s="34">
+        <v>4</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="24" t="s">
@@ -2530,14 +2747,18 @@
       <c r="D15" s="15">
         <v>0</v>
       </c>
-      <c r="E15" s="34"/>
+      <c r="E15" s="34">
+        <v>4</v>
+      </c>
       <c r="F15" s="21">
         <v>2</v>
       </c>
       <c r="G15" s="15">
         <v>0</v>
       </c>
-      <c r="H15" s="34"/>
+      <c r="H15" s="34">
+        <v>3</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="24" t="s">
@@ -2552,14 +2773,18 @@
       <c r="D16" s="15">
         <v>0</v>
       </c>
-      <c r="E16" s="34"/>
+      <c r="E16" s="34">
+        <v>6</v>
+      </c>
       <c r="F16" s="21">
         <v>2</v>
       </c>
       <c r="G16" s="15">
         <v>0</v>
       </c>
-      <c r="H16" s="34"/>
+      <c r="H16" s="34">
+        <v>4</v>
+      </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="24" t="s">
@@ -2574,14 +2799,18 @@
       <c r="D17" s="15">
         <v>0</v>
       </c>
-      <c r="E17" s="34"/>
+      <c r="E17" s="34">
+        <v>8</v>
+      </c>
       <c r="F17" s="21">
         <v>4</v>
       </c>
       <c r="G17" s="15">
         <v>0</v>
       </c>
-      <c r="H17" s="34"/>
+      <c r="H17" s="34">
+        <v>10</v>
+      </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="24" t="s">
@@ -2603,7 +2832,9 @@
       <c r="G18" s="15">
         <v>0.5</v>
       </c>
-      <c r="H18" s="34"/>
+      <c r="H18" s="34">
+        <v>1</v>
+      </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="24" t="s">
@@ -2618,14 +2849,18 @@
       <c r="D19" s="15">
         <v>0</v>
       </c>
-      <c r="E19" s="34"/>
+      <c r="E19" s="34">
+        <v>4</v>
+      </c>
       <c r="F19" s="21">
         <v>2</v>
       </c>
       <c r="G19" s="15">
         <v>0</v>
       </c>
-      <c r="H19" s="34"/>
+      <c r="H19" s="34">
+        <v>4</v>
+      </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="24" t="s">
@@ -2640,14 +2875,18 @@
       <c r="D20" s="15">
         <v>0</v>
       </c>
-      <c r="E20" s="34"/>
+      <c r="E20" s="34">
+        <v>4</v>
+      </c>
       <c r="F20" s="21">
         <v>2</v>
       </c>
       <c r="G20" s="15">
         <v>0</v>
       </c>
-      <c r="H20" s="34"/>
+      <c r="H20" s="34">
+        <v>4</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="24" t="s">
@@ -2662,14 +2901,18 @@
       <c r="D21" s="15">
         <v>0</v>
       </c>
-      <c r="E21" s="34"/>
+      <c r="E21" s="34">
+        <v>1</v>
+      </c>
       <c r="F21" s="21">
         <v>2</v>
       </c>
       <c r="G21" s="15">
         <v>0</v>
       </c>
-      <c r="H21" s="34"/>
+      <c r="H21" s="34">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="24" t="s">
@@ -2734,7 +2977,7 @@
       </c>
       <c r="E26" s="6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="F26" s="52">
         <f t="shared" si="0"/>
@@ -2746,7 +2989,7 @@
       </c>
       <c r="H26" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2760,7 +3003,7 @@
       </c>
       <c r="D27" s="64">
         <f>D26+E26</f>
-        <v>18.399999999999999</v>
+        <v>51.4</v>
       </c>
       <c r="E27" s="64"/>
       <c r="F27" s="52">
@@ -2769,7 +3012,7 @@
       </c>
       <c r="G27" s="64">
         <f>G26+H26</f>
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="H27" s="64"/>
     </row>
@@ -2808,7 +3051,7 @@
       </c>
       <c r="D30" s="49">
         <f>D27+G27</f>
-        <v>33.4</v>
+        <v>97.4</v>
       </c>
       <c r="E30" s="41"/>
       <c r="F30" s="43"/>
@@ -2845,7 +3088,9 @@
       <c r="B33" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="C33" s="68"/>
+      <c r="C33" s="68" t="s">
+        <v>72</v>
+      </c>
       <c r="D33" s="69"/>
       <c r="E33" s="69"/>
       <c r="F33" s="69"/>
@@ -2857,7 +3102,9 @@
       <c r="B34" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="C34" s="68"/>
+      <c r="C34" s="68" t="s">
+        <v>73</v>
+      </c>
       <c r="D34" s="69"/>
       <c r="E34" s="69"/>
       <c r="F34" s="69"/>
@@ -2869,7 +3116,9 @@
       <c r="B35" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="C35" s="70"/>
+      <c r="C35" s="70" t="s">
+        <v>74</v>
+      </c>
       <c r="D35" s="71"/>
       <c r="E35" s="71"/>
       <c r="F35" s="71"/>
@@ -2906,7 +3155,9 @@
       <c r="B38" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="C38" s="68"/>
+      <c r="C38" s="68" t="s">
+        <v>75</v>
+      </c>
       <c r="D38" s="69"/>
       <c r="E38" s="69"/>
       <c r="F38" s="69"/>
@@ -2918,7 +3169,9 @@
       <c r="B39" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="C39" s="68"/>
+      <c r="C39" s="68" t="s">
+        <v>76</v>
+      </c>
       <c r="D39" s="69"/>
       <c r="E39" s="69"/>
       <c r="F39" s="69"/>
@@ -2930,7 +3183,9 @@
       <c r="B40" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="C40" s="70"/>
+      <c r="C40" s="70" t="s">
+        <v>77</v>
+      </c>
       <c r="D40" s="71"/>
       <c r="E40" s="71"/>
       <c r="F40" s="71"/>
@@ -3024,7 +3279,7 @@
     </row>
     <row r="4" spans="1:8" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="60"/>
-      <c r="B4" s="72"/>
+      <c r="B4" s="73"/>
       <c r="C4" s="14" t="s">
         <v>7</v>
       </c>
@@ -3534,7 +3789,7 @@
       <c r="B35" s="54" t="s">
         <v>70</v>
       </c>
-      <c r="C35" s="70"/>
+      <c r="C35" s="72"/>
       <c r="D35" s="71"/>
       <c r="E35" s="71"/>
       <c r="F35" s="71"/>
@@ -3595,7 +3850,7 @@
       <c r="B40" s="54" t="s">
         <v>70</v>
       </c>
-      <c r="C40" s="70"/>
+      <c r="C40" s="72"/>
       <c r="D40" s="71"/>
       <c r="E40" s="71"/>
       <c r="F40" s="71"/>

</xml_diff>